<commit_message>
proj: Add project gantt time line
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/isa.xlsx
+++ b/docs/isa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\uni\vmicro16\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ED801DF-6741-4CB5-B16C-257EBFCE3C9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A36342-E13B-42BF-BF69-B72609D57AFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{D926F85F-F5FA-444C-8EB3-6C2AF9618F1A}"/>
   </bookViews>
@@ -538,7 +538,14 @@
     <xf numFmtId="49" fontId="8" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -548,13 +555,6 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BB6428-591B-4A36-AF5A-896D3360B183}">
   <dimension ref="A5:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,10 +914,10 @@
       <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="7" t="s">
         <v>100</v>
       </c>
@@ -928,11 +928,11 @@
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="10" t="s">
         <v>101</v>
       </c>
@@ -946,10 +946,10 @@
       <c r="C8" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="7" t="s">
         <v>98</v>
       </c>
@@ -962,11 +962,11 @@
       <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="8"/>
       <c r="G9" s="2"/>
     </row>
@@ -1190,10 +1190,10 @@
       <c r="C20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="8" t="s">
         <v>38</v>
       </c>
@@ -1377,10 +1377,10 @@
       <c r="C29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="14"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="5" t="s">
         <v>82</v>
       </c>
@@ -1396,10 +1396,10 @@
       <c r="C30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="16"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="3" t="s">
         <v>56</v>
       </c>
@@ -1415,10 +1415,10 @@
       <c r="C31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="16"/>
+      <c r="E31" s="12"/>
       <c r="F31" s="3" t="s">
         <v>57</v>
       </c>
@@ -1434,10 +1434,10 @@
       <c r="C32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="16"/>
+      <c r="E32" s="12"/>
       <c r="F32" s="3" t="s">
         <v>58</v>
       </c>
@@ -1453,10 +1453,10 @@
       <c r="C33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="16"/>
+      <c r="E33" s="12"/>
       <c r="F33" s="3" t="s">
         <v>59</v>
       </c>
@@ -1472,10 +1472,10 @@
       <c r="C34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="16"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="3" t="s">
         <v>61</v>
       </c>
@@ -1491,10 +1491,10 @@
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E35" s="16"/>
+      <c r="E35" s="12"/>
       <c r="F35" s="3" t="s">
         <v>63</v>
       </c>
@@ -1509,10 +1509,10 @@
       <c r="C36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="16"/>
+      <c r="E36" s="12"/>
       <c r="F36" s="3" t="s">
         <v>89</v>
       </c>
@@ -1527,10 +1527,10 @@
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="16"/>
+      <c r="E37" s="12"/>
       <c r="F37" s="3" t="s">
         <v>66</v>
       </c>
@@ -1545,10 +1545,10 @@
       <c r="C38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="16"/>
+      <c r="E38" s="12"/>
       <c r="F38" s="3" t="s">
         <v>68</v>
       </c>
@@ -1603,10 +1603,10 @@
       <c r="C41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="E41" s="17"/>
+      <c r="E41" s="14"/>
       <c r="F41" s="9" t="s">
         <v>96</v>
       </c>
@@ -1619,6 +1619,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D29:E29"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
@@ -1630,11 +1635,6 @@
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cpu: decoder, registers in pipeline
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/isa.xlsx
+++ b/docs/isa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\uni\vmicro16\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A36342-E13B-42BF-BF69-B72609D57AFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580FF8D2-AC20-45C8-8A64-4922FE28D6A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{D926F85F-F5FA-444C-8EB3-6C2AF9618F1A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="110">
   <si>
     <t>NOP</t>
   </si>
@@ -357,13 +357,16 @@
   </si>
   <si>
     <t>Rd &lt;= sRd - sRa + AAAA</t>
+  </si>
+  <si>
+    <t>Timing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,8 +433,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,6 +461,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -519,14 +534,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="4"/>
@@ -538,14 +554,7 @@
     <xf numFmtId="49" fontId="8" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -555,8 +564,17 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="5" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BB6428-591B-4A36-AF5A-896D3360B183}">
   <dimension ref="A5:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,10 +932,10 @@
       <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="7" t="s">
         <v>100</v>
       </c>
@@ -928,11 +946,11 @@
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="10" t="s">
         <v>101</v>
       </c>
@@ -946,10 +964,10 @@
       <c r="C8" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="7" t="s">
         <v>98</v>
       </c>
@@ -962,11 +980,11 @@
       <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="8"/>
       <c r="G9" s="2"/>
     </row>
@@ -989,7 +1007,9 @@
       <c r="F10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="18" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
@@ -1010,7 +1030,9 @@
       <c r="F11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="18" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -1190,10 +1212,10 @@
       <c r="C20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="15"/>
+      <c r="E20" s="12"/>
       <c r="F20" s="8" t="s">
         <v>38</v>
       </c>
@@ -1281,7 +1303,9 @@
       <c r="F24" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="18" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
@@ -1365,7 +1389,9 @@
       <c r="F28" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G28" s="2"/>
+      <c r="G28" s="18" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
@@ -1377,10 +1403,10 @@
       <c r="C29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="17"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="5" t="s">
         <v>82</v>
       </c>
@@ -1396,10 +1422,10 @@
       <c r="C30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="12"/>
+      <c r="E30" s="16"/>
       <c r="F30" s="3" t="s">
         <v>56</v>
       </c>
@@ -1415,10 +1441,10 @@
       <c r="C31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="16"/>
       <c r="F31" s="3" t="s">
         <v>57</v>
       </c>
@@ -1434,10 +1460,10 @@
       <c r="C32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="12"/>
+      <c r="E32" s="16"/>
       <c r="F32" s="3" t="s">
         <v>58</v>
       </c>
@@ -1453,10 +1479,10 @@
       <c r="C33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="12"/>
+      <c r="E33" s="16"/>
       <c r="F33" s="3" t="s">
         <v>59</v>
       </c>
@@ -1472,10 +1498,10 @@
       <c r="C34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="12"/>
+      <c r="E34" s="16"/>
       <c r="F34" s="3" t="s">
         <v>61</v>
       </c>
@@ -1491,10 +1517,10 @@
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E35" s="12"/>
+      <c r="E35" s="16"/>
       <c r="F35" s="3" t="s">
         <v>63</v>
       </c>
@@ -1509,10 +1535,10 @@
       <c r="C36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="12"/>
+      <c r="E36" s="16"/>
       <c r="F36" s="3" t="s">
         <v>89</v>
       </c>
@@ -1527,10 +1553,10 @@
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="12"/>
+      <c r="E37" s="16"/>
       <c r="F37" s="3" t="s">
         <v>66</v>
       </c>
@@ -1545,10 +1571,10 @@
       <c r="C38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="12"/>
+      <c r="E38" s="16"/>
       <c r="F38" s="3" t="s">
         <v>68</v>
       </c>
@@ -1603,10 +1629,10 @@
       <c r="C41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E41" s="14"/>
+      <c r="E41" s="17"/>
       <c r="F41" s="9" t="s">
         <v>96</v>
       </c>
@@ -1619,11 +1645,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D29:E29"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
@@ -1635,6 +1656,11 @@
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cpu: hardware multiplier optional
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/isa.xlsx
+++ b/docs/isa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\uni\vmicro16\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\uni\vmicro16\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4A1E9B-4D8A-4548-A496-F047AA77ABC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0789B65A-0689-47F4-8EA4-7B64E9D83BCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9210" xr2:uid="{D926F85F-F5FA-444C-8EB3-6C2AF9618F1A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="115">
   <si>
     <t>NOP</t>
   </si>
@@ -360,6 +360,21 @@
   </si>
   <si>
     <t>Timing</t>
+  </si>
+  <si>
+    <t>MULT</t>
+  </si>
+  <si>
+    <t>01011</t>
+  </si>
+  <si>
+    <t>Rd &lt;= uRd * uRa</t>
+  </si>
+  <si>
+    <t>HALT</t>
+  </si>
+  <si>
+    <t>01100</t>
   </si>
 </sst>
 </file>
@@ -555,14 +570,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -572,6 +580,13 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -891,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BB6428-591B-4A36-AF5A-896D3360B183}">
-  <dimension ref="A5:G42"/>
+  <dimension ref="A5:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,10 +947,10 @@
       <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="7" t="s">
         <v>100</v>
       </c>
@@ -946,11 +961,11 @@
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="10" t="s">
         <v>101</v>
       </c>
@@ -964,10 +979,10 @@
       <c r="C8" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="7" t="s">
         <v>98</v>
       </c>
@@ -980,11 +995,11 @@
       <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="8"/>
       <c r="G9" s="2"/>
     </row>
@@ -1212,10 +1227,10 @@
       <c r="C20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="8" t="s">
         <v>38</v>
       </c>
@@ -1403,10 +1418,10 @@
       <c r="C29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="15"/>
       <c r="F29" s="5" t="s">
         <v>82</v>
       </c>
@@ -1422,10 +1437,10 @@
       <c r="C30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="13"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="3" t="s">
         <v>56</v>
       </c>
@@ -1441,10 +1456,10 @@
       <c r="C31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="13"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="3" t="s">
         <v>57</v>
       </c>
@@ -1460,10 +1475,10 @@
       <c r="C32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="13"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="3" t="s">
         <v>58</v>
       </c>
@@ -1479,10 +1494,10 @@
       <c r="C33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="13"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="3" t="s">
         <v>59</v>
       </c>
@@ -1498,10 +1513,10 @@
       <c r="C34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="13"/>
+      <c r="E34" s="17"/>
       <c r="F34" s="3" t="s">
         <v>61</v>
       </c>
@@ -1517,10 +1532,10 @@
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="3" t="s">
         <v>63</v>
       </c>
@@ -1535,10 +1550,10 @@
       <c r="C36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="13"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="3" t="s">
         <v>89</v>
       </c>
@@ -1553,10 +1568,10 @@
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="13"/>
+      <c r="E37" s="17"/>
       <c r="F37" s="3" t="s">
         <v>66</v>
       </c>
@@ -1571,10 +1586,10 @@
       <c r="C38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="13"/>
+      <c r="E38" s="17"/>
       <c r="F38" s="3" t="s">
         <v>68</v>
       </c>
@@ -1620,47 +1635,85 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="15" t="s">
+      <c r="C43" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="9" t="s">
+      <c r="E43" s="18"/>
+      <c r="F43" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G41"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="G43"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D29:E29"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D43:E43"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
m: start of impl for lwex/swex
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/isa.xlsx
+++ b/docs/isa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\uni\vmicro16\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\uni\vmicro16\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0789B65A-0689-47F4-8EA4-7B64E9D83BCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB49DC1-368F-4D69-A55E-9AD25F948274}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9210" xr2:uid="{D926F85F-F5FA-444C-8EB3-6C2AF9618F1A}"/>
+    <workbookView xWindow="3570" yWindow="2985" windowWidth="14025" windowHeight="13575" xr2:uid="{D926F85F-F5FA-444C-8EB3-6C2AF9618F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="115">
   <si>
     <t>NOP</t>
   </si>
@@ -302,30 +302,15 @@
     <t>Z=1 or (S != O)</t>
   </si>
   <si>
-    <t>MOVI_LARGE</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>14:12</t>
   </si>
   <si>
     <t>11:0</t>
   </si>
   <si>
-    <t>i12</t>
-  </si>
-  <si>
-    <t>Rd &lt;= i12</t>
-  </si>
-  <si>
-    <t>TODO: high/low byte addressing</t>
-  </si>
-  <si>
     <t>extended immediate</t>
   </si>
   <si>
@@ -375,13 +360,29 @@
   </si>
   <si>
     <t>01100</t>
+  </si>
+  <si>
+    <t>01101</t>
+  </si>
+  <si>
+    <t>01110</t>
+  </si>
+  <si>
+    <t>LWEX</t>
+  </si>
+  <si>
+    <t>SWEX</t>
+  </si>
+  <si>
+    <t>RAM[Ra+s5] &lt;= Rd
+Rd &lt;= 0|1 if success</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,13 +415,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -555,7 +549,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -563,30 +557,32 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -908,15 +904,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BB6428-591B-4A36-AF5A-896D3360B183}">
   <dimension ref="A5:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:E29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
     <col min="2" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="23.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -935,7 +931,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -947,12 +943,12 @@
       <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -961,30 +957,30 @@
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="10" t="s">
-        <v>101</v>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -995,11 +991,11 @@
       <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="8"/>
       <c r="G9" s="2"/>
     </row>
@@ -1022,8 +1018,8 @@
       <c r="F10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>109</v>
+      <c r="G10" s="10" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1045,8 +1041,8 @@
       <c r="F11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>109</v>
+      <c r="G11" s="10" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1227,10 +1223,10 @@
       <c r="C20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="13"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="8" t="s">
         <v>38</v>
       </c>
@@ -1271,7 +1267,7 @@
         <v>12</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>44</v>
@@ -1292,7 +1288,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>46</v>
@@ -1301,7 +1297,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>39</v>
@@ -1313,14 +1309,12 @@
         <v>12</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>109</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -1357,7 +1351,7 @@
         <v>12</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>48</v>
@@ -1378,7 +1372,7 @@
         <v>12</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>50</v>
@@ -1387,7 +1381,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>42</v>
@@ -1399,14 +1393,12 @@
         <v>12</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>109</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -1418,10 +1410,10 @@
       <c r="C29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="15"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="5" t="s">
         <v>82</v>
       </c>
@@ -1437,10 +1429,10 @@
       <c r="C30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="17"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="3" t="s">
         <v>56</v>
       </c>
@@ -1456,10 +1448,10 @@
       <c r="C31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="17"/>
+      <c r="E31" s="12"/>
       <c r="F31" s="3" t="s">
         <v>57</v>
       </c>
@@ -1475,10 +1467,10 @@
       <c r="C32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="17"/>
+      <c r="E32" s="12"/>
       <c r="F32" s="3" t="s">
         <v>58</v>
       </c>
@@ -1494,10 +1486,10 @@
       <c r="C33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="17"/>
+      <c r="E33" s="12"/>
       <c r="F33" s="3" t="s">
         <v>59</v>
       </c>
@@ -1513,10 +1505,10 @@
       <c r="C34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="17"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="3" t="s">
         <v>61</v>
       </c>
@@ -1532,10 +1524,10 @@
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E35" s="17"/>
+      <c r="E35" s="12"/>
       <c r="F35" s="3" t="s">
         <v>63</v>
       </c>
@@ -1550,10 +1542,10 @@
       <c r="C36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="17"/>
+      <c r="E36" s="12"/>
       <c r="F36" s="3" t="s">
         <v>89</v>
       </c>
@@ -1568,10 +1560,10 @@
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="17"/>
+      <c r="E37" s="12"/>
       <c r="F37" s="3" t="s">
         <v>66</v>
       </c>
@@ -1586,10 +1578,10 @@
       <c r="C38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="17"/>
+      <c r="E38" s="12"/>
       <c r="F38" s="3" t="s">
         <v>68</v>
       </c>
@@ -1636,10 +1628,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>11</v>
@@ -1651,15 +1643,15 @@
         <v>8</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>8</v>
@@ -1673,47 +1665,63 @@
       <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="9" t="s">
-        <v>96</v>
+      <c r="A43" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>97</v>
+    <row r="44" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D29:E29"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D43:E43"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sw: temp fix for losing bp_offset somehow
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/isa.xlsx
+++ b/docs/isa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\uni\vmicro16\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB49DC1-368F-4D69-A55E-9AD25F948274}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A631B51-2E96-4777-8454-B57EAEC3F185}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="2985" windowWidth="14025" windowHeight="13575" xr2:uid="{D926F85F-F5FA-444C-8EB3-6C2AF9618F1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D926F85F-F5FA-444C-8EB3-6C2AF9618F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="116">
   <si>
     <t>NOP</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>01010</t>
-  </si>
-  <si>
-    <t>Rd &lt;= Imm8 == SZO ? 1 : 0</t>
   </si>
   <si>
     <t>Z=1 or (S != O)</t>
@@ -376,6 +373,12 @@
   <si>
     <t>RAM[Ra+s5] &lt;= Rd
 Rd &lt;= 0|1 if success</t>
+  </si>
+  <si>
+    <t>Imm8</t>
+  </si>
+  <si>
+    <t>Rd &lt;= (Imm8 _f_ SZO) ? 1 : 0</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -542,6 +545,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -551,7 +580,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="4"/>
@@ -563,11 +592,9 @@
     <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -579,9 +606,17 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -904,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BB6428-591B-4A36-AF5A-896D3360B183}">
   <dimension ref="A5:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +966,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -948,7 +983,7 @@
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -963,24 +998,24 @@
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>92</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -1019,7 +1054,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1042,7 +1077,7 @@
         <v>36</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1267,7 +1302,7 @@
         <v>12</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>44</v>
@@ -1288,7 +1323,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>46</v>
@@ -1297,7 +1332,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>39</v>
@@ -1309,10 +1344,10 @@
         <v>12</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G24" s="2"/>
     </row>
@@ -1351,7 +1386,7 @@
         <v>12</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>48</v>
@@ -1372,7 +1407,7 @@
         <v>12</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>50</v>
@@ -1381,7 +1416,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>42</v>
@@ -1393,10 +1428,10 @@
         <v>12</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -1429,10 +1464,10 @@
       <c r="C30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="12"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="3" t="s">
         <v>56</v>
       </c>
@@ -1448,10 +1483,10 @@
       <c r="C31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="18"/>
       <c r="F31" s="3" t="s">
         <v>57</v>
       </c>
@@ -1467,10 +1502,10 @@
       <c r="C32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="12"/>
+      <c r="E32" s="18"/>
       <c r="F32" s="3" t="s">
         <v>58</v>
       </c>
@@ -1486,10 +1521,10 @@
       <c r="C33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="12"/>
+      <c r="E33" s="18"/>
       <c r="F33" s="3" t="s">
         <v>59</v>
       </c>
@@ -1505,10 +1540,10 @@
       <c r="C34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="12"/>
+      <c r="E34" s="18"/>
       <c r="F34" s="3" t="s">
         <v>61</v>
       </c>
@@ -1524,10 +1559,10 @@
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E35" s="12"/>
+      <c r="E35" s="18"/>
       <c r="F35" s="3" t="s">
         <v>63</v>
       </c>
@@ -1542,12 +1577,12 @@
       <c r="C36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="12"/>
+      <c r="E36" s="18"/>
       <c r="F36" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1560,10 +1595,10 @@
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="12"/>
+      <c r="E37" s="18"/>
       <c r="F37" s="3" t="s">
         <v>66</v>
       </c>
@@ -1578,10 +1613,10 @@
       <c r="C38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="12"/>
+      <c r="E38" s="18"/>
       <c r="F38" s="3" t="s">
         <v>68</v>
       </c>
@@ -1616,22 +1651,20 @@
       <c r="C40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="D40" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E40" s="20"/>
       <c r="F40" s="8" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>11</v>
@@ -1643,15 +1676,15 @@
         <v>8</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>8</v>
@@ -1665,53 +1698,49 @@
       <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G43"/>
+    </row>
+    <row r="44" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B44" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="17" t="s">
+      <c r="C44" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G43"/>
-    </row>
-    <row r="44" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+      <c r="F44" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>114</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D29:E29"/>
+  <mergeCells count="16">
+    <mergeCell ref="D40:E40"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
@@ -1722,6 +1751,11 @@
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
soc: use ram instead of regs for exflags
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/isa.xlsx
+++ b/docs/isa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\uni\vmicro16\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7146D761-7773-492C-B5B2-1AEEA3FA759D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839CEE58-166C-4B5E-A320-0F7A681C517B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6210" yWindow="5730" windowWidth="14025" windowHeight="13575" xr2:uid="{D926F85F-F5FA-444C-8EB3-6C2AF9618F1A}"/>
   </bookViews>
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BB6428-591B-4A36-AF5A-896D3360B183}">
   <dimension ref="A5:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>